<commit_message>
Add elegibility at each day, every cohort
</commit_message>
<xml_diff>
--- a/results/table1_coh_1.xlsx
+++ b/results/table1_coh_1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,7 +823,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>MV initiated in the cohort day, n (%)</t>
+          <t>Mechanical Ventilation (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
@@ -836,19 +836,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1214 (49.6)</t>
+          <t>1392 (56.9)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5432 (51.2)</t>
+          <t>6318 (59.6)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>RRT initiated in the cohort day, n (%)</t>
+          <t>RRT (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
@@ -861,19 +861,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>233 (9.5)</t>
+          <t>371 (15.2)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>507 (4.8)</t>
+          <t>1027 (9.7)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor initiated in the cohort day, n (%)</t>
+          <t>Vasopressors (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -886,24 +886,24 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1004 (41.0)</t>
+          <t>1181 (48.2)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5094 (48.0)</t>
+          <t>5932 (55.9)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Mechanical Ventilation (whole stay), n (%)</t>
+          <t>Insulin Transfusion (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1392 (56.9)</t>
+          <t>1502 (61.4)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -923,12 +923,12 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>RRT (whole stay), n (%)</t>
+          <t>Blood Transufusion (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -936,24 +936,24 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>371 (15.2)</t>
+          <t>256 (10.5)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1027 (9.7)</t>
+          <t>1296 (12.2)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Vasopressors (whole stay), n (%)</t>
+          <t>Fluids Received (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -961,19 +961,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1181 (48.2)</t>
+          <t>2385 (97.4)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5932 (55.9)</t>
+          <t>10357 (97.7)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Insulin Transfusion (whole stay), n (%)</t>
+          <t>Hypertension, n (%)</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -986,19 +986,19 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1502 (61.4)</t>
+          <t>1704 (69.6)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6318 (59.6)</t>
+          <t>6977 (65.8)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Blood Transufusion (whole stay), n (%)</t>
+          <t>Congestive Heart Failure, n (%)</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
@@ -1011,19 +1011,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>256 (10.5)</t>
+          <t>915 (37.4)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1296 (12.2)</t>
+          <t>3851 (36.3)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Fluids Received (whole stay), n (%)</t>
+          <t>COPD, n (%)</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -1036,19 +1036,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2385 (97.4)</t>
+          <t>562 (23.0)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10357 (97.7)</t>
+          <t>2623 (24.7)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Hypertension, n (%)</t>
+          <t>Asthma, n (%)</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
@@ -1061,19 +1061,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1704 (69.6)</t>
+          <t>34 (1.4)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6977 (65.8)</t>
+          <t>152 (1.4)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Congestive Heart Failure, n (%)</t>
+          <t>Coronary Artery Disease, n (%)</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
@@ -1086,19 +1086,19 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>915 (37.4)</t>
+          <t>754 (30.8)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3851 (36.3)</t>
+          <t>4137 (39.0)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>COPD, n (%)</t>
+          <t>CKD Stage, n (%)</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
@@ -1111,87 +1111,69 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>562 (23.0)</t>
+          <t>3 (0.1)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2623 (24.7)</t>
+          <t>2 (0.0)</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Asthma, n (%)</t>
-        </is>
-      </c>
+      <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>34 (1.4)</t>
+          <t>19 (0.8)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>152 (1.4)</t>
+          <t>68 (0.6)</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Coronary Artery Disease, n (%)</t>
-        </is>
-      </c>
+      <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>754 (30.8)</t>
+          <t>161 (6.6)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4137 (39.0)</t>
+          <t>532 (5.0)</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>CKD Stage, n (%)</t>
-        </is>
-      </c>
+      <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3 (0.1)</t>
+          <t>62 (2.5)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2 (0.0)</t>
+          <t>185 (1.7)</t>
         </is>
       </c>
     </row>
@@ -1199,18 +1181,18 @@
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>19 (0.8)</t>
+          <t>264 (10.8)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>68 (0.6)</t>
+          <t>461 (4.3)</t>
         </is>
       </c>
     </row>
@@ -1218,37 +1200,43 @@
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>Absent</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>161 (6.6)</t>
+          <t>1939 (79.2)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>532 (5.0)</t>
+          <t>9355 (88.2)</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n"/>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes Type, n (%)</t>
+        </is>
+      </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>62 (2.5)</t>
+          <t>75 (3.1)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>185 (1.7)</t>
+          <t>300 (2.8)</t>
         </is>
       </c>
     </row>
@@ -1256,18 +1244,18 @@
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>264 (10.8)</t>
+          <t>986 (40.3)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>461 (4.3)</t>
+          <t>2962 (27.9)</t>
         </is>
       </c>
     </row>
@@ -1281,19 +1269,19 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1939 (79.2)</t>
+          <t>1387 (56.7)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9355 (88.2)</t>
+          <t>7341 (69.2)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Diabetes Type, n (%)</t>
+          <t>Connective Tissue Disease, n (%)</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
@@ -1306,57 +1294,69 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>75 (3.1)</t>
+          <t>117 (4.8)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>300 (2.8)</t>
+          <t>472 (4.5)</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n"/>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Pneumonia, n (%)</t>
+        </is>
+      </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>986 (40.3)</t>
+          <t>139 (5.7)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2962 (27.9)</t>
+          <t>507 (4.8)</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n"/>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Urinary Tract Infection, n (%)</t>
+        </is>
+      </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1387 (56.7)</t>
+          <t>15 (0.6)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>7341 (69.2)</t>
+          <t>84 (0.8)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Connective Tissue Disease, n (%)</t>
+          <t>Biliary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
@@ -1369,19 +1369,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>117 (4.8)</t>
+          <t>2 (0.1)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>472 (4.5)</t>
+          <t>20 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Pneumonia, n (%)</t>
+          <t>Skin Infection, n (%)</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
@@ -1394,24 +1394,24 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>139 (5.7)</t>
+          <t>4 (0.2)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>507 (4.8)</t>
+          <t>21 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Urinary Tract Infection, n (%)</t>
+          <t>MV initiated in day 1, n (%)</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1419,24 +1419,24 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15 (0.6)</t>
+          <t>1214 (49.6)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>84 (0.8)</t>
+          <t>5432 (51.2)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Biliary Tract Infection, n (%)</t>
+          <t>RRT initiated in day 1, n (%)</t>
         </is>
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1444,24 +1444,24 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2 (0.1)</t>
+          <t>233 (9.5)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>20 (0.2)</t>
+          <t>507 (4.8)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Skin Infection, n (%)</t>
+          <t>Vasopressor initiated in day 1, n (%)</t>
         </is>
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1469,976 +1469,1201 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4 (0.2)</t>
+          <t>1004 (41.0)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>21 (0.2)</t>
+          <t>5094 (48.0)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Age, median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B46" s="1" t="inlineStr"/>
+          <t>MV initiated in day 2, n (%)</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>64 [52,75]</t>
+          <t>77 (3.1)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>68 [58,78]</t>
+          <t>441 (4.2)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B47" s="1" t="inlineStr"/>
+          <t>RRT initiated in day 2, n (%)</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C47" t="n">
-        <v>10855</v>
+        <v>0</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.23 [3.23,8.99]</t>
+          <t>60 (2.5)</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5.38 [3.29,9.38]</t>
+          <t>208 (2.0)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B48" s="1" t="inlineStr"/>
+          <t>Vasopressor initiated in day 2, n (%)</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C48" t="n">
-        <v>2196</v>
+        <v>0</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.17 [2.83,7.71]</t>
+          <t>80 (3.3)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.08 [2.79,7.17]</t>
+          <t>405 (3.8)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B49" s="1" t="inlineStr"/>
+          <t>MV initiated in day 3, n (%)</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C49" t="n">
-        <v>10855</v>
+        <v>0</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10.00 [6.00,19.00]</t>
+          <t>41 (1.7)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>11.00 [6.00,18.75]</t>
+          <t>221 (2.1)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B50" s="1" t="inlineStr"/>
+          <t>RRT initiated in day 3, n (%)</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C50" t="n">
-        <v>2196</v>
+        <v>0</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12.00 [7.00,20.00]</t>
+          <t>30 (1.2)</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>11.00 [7.00,18.00]</t>
+          <t>124 (1.2)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B51" s="1" t="inlineStr"/>
+          <t>Vasopressor initiated in day 3, n (%)</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>39 (1.6)</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>200 (1.9)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>SOFA Score (admission), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B52" s="1" t="inlineStr"/>
+          <t>MV initiated in day 4, n (%)</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>31 (1.3)</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>5 [3,8]</t>
+          <t>107 (1.0)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B53" s="1" t="inlineStr"/>
+          <t>RRT initiated in day 4, n (%)</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C53" t="n">
-        <v>4756</v>
+        <v>0</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>19 (0.8)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>59 (0.6)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B54" s="1" t="inlineStr"/>
+          <t>Vasopressor initiated in day 4, n (%)</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C54" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>28 (1.1)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>104 (1.0)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
+          <t>Age, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B55" s="1" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>5163</v>
+        <v>0</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>64 [52,75]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>68 [58,78]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
+          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>18</v>
+        <v>10855</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>5.23 [3.23,8.99]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>5.38 [3.29,9.38]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
+          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr"/>
       <c r="C57" t="n">
-        <v>22</v>
+        <v>2196</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>4.17 [2.83,7.71]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>4.08 [2.79,7.17]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
+          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr"/>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>10855</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>10.00 [6.00,19.00]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>11.00 [6.00,18.75]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>SOFA (day), median [Q1,Q3]</t>
+          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>15</v>
+        <v>2196</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>12.00 [7.00,20.00]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>11.00 [7.00,18.00]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Respiratory (day), median [Q1,Q3]</t>
+          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B60" s="1" t="inlineStr"/>
       <c r="C60" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.0 [0.0,2.0]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Coagulation (day), median [Q1,Q3]</t>
+          <t>SOFA Score (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B61" s="1" t="inlineStr"/>
       <c r="C61" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>5 [3,8]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Liver (day), median [Q1,Q3]</t>
+          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr"/>
       <c r="C62" t="n">
-        <v>15</v>
+        <v>4756</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Cardiovascular (day), median [Q1,Q3]</t>
+          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B63" s="1" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>SOFA: CNS (day), median [Q1,Q3]</t>
+          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B64" s="1" t="inlineStr"/>
       <c r="C64" t="n">
-        <v>15</v>
+        <v>5163</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Renal (day), median [Q1,Q3]</t>
+          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B65" s="1" t="inlineStr"/>
       <c r="C65" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (day), median [Q1,Q3]</t>
+          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr"/>
       <c r="C66" t="n">
-        <v>4731</v>
+        <v>22</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>729 [246,1498]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>650 [210,1463]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
+          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B67" s="1" t="inlineStr"/>
       <c r="C67" t="n">
-        <v>309</v>
+        <v>1</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2648 [994,5920]</t>
+          <t>1 [0,2]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2369 [817,5431]</t>
+          <t>1 [0,2]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
+          <t>SOFA (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B68" s="1" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>309</v>
+        <v>15</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>506.2 [226.7,963.1]</t>
+          <t>5.0 [3.0,8.0]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>477.0 [204.8,905.2]</t>
+          <t>5.0 [3.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>FiO2 (mean %), median [Q1,Q3]</t>
+          <t>SOFA: Respiratory (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B69" s="1" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>7672</v>
+        <v>15</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>50 [40,60]</t>
+          <t>0.0 [0.0,2.0]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>50 [42,65]</t>
+          <t>1.0 [0.0,2.0]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>MV_time_abs_hours, median [Q1,Q3]</t>
+          <t>SOFA: Coagulation (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B70" s="1" t="inlineStr"/>
       <c r="C70" t="n">
-        <v>5341</v>
+        <v>15</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>39.0 [17.0,86.2]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>32.0 [15.0,76.0]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>SOFA: Liver (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr"/>
       <c r="C71" t="n">
-        <v>5341</v>
+        <v>15</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.30 [0.14,0.50]</t>
+          <t>0.0 [0.0,0.0]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.26 [0.13,0.45]</t>
+          <t>0.0 [0.0,0.0]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>SOFA: Cardiovascular (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr"/>
       <c r="C72" t="n">
-        <v>5341</v>
+        <v>15</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2.0 [1.0,8.0]</t>
+          <t>1.0 [1.0,3.0]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3.0 [1.0,8.0]</t>
+          <t>1.0 [1.0,3.0]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>SOFA: CNS (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr"/>
       <c r="C73" t="n">
-        <v>11653</v>
+        <v>15</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>16.0 [4.0,41.0]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>25.0 [5.5,63.0]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>SOFA: Renal (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr"/>
       <c r="C74" t="n">
-        <v>5827</v>
+        <v>15</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3.0 [1.0,12.0]</t>
+          <t>1.0 [0.0,2.0]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3.0 [1.0,10.0]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>VP_time_abs_hours, median [Q1,Q3]</t>
+          <t>Fluids Volume (day), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr"/>
       <c r="C75" t="n">
-        <v>5827</v>
+        <v>4731</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>29.0 [10.0,65.0]</t>
+          <t>729 [246,1498]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>29.0 [11.0,62.0]</t>
+          <t>650 [210,1463]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr"/>
       <c r="C76" t="n">
-        <v>5827</v>
+        <v>309</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.23 [0.08,0.48]</t>
+          <t>2648 [994,5920]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0.25 [0.09,0.47]</t>
+          <t>2369 [817,5431]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Respiratory Rate (mean), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr"/>
       <c r="C77" t="n">
-        <v>24</v>
+        <v>309</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>19.4 [17.0,22.6]</t>
+          <t>506.2 [226.7,963.1]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>19.1 [16.8,22.0]</t>
+          <t>477.0 [204.8,905.2]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>Mean Blood Pressure (mean), median [Q1,Q3]</t>
+          <t>FiO2 (mean %), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr"/>
       <c r="C78" t="n">
-        <v>18</v>
+        <v>7672</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>77.5 [71.1,85.4]</t>
+          <t>50 [40,60]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>74.7 [69.4,81.6]</t>
+          <t>50 [42,65]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
+          <t>MV_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr"/>
       <c r="C79" t="n">
-        <v>693</v>
+        <v>5341</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.3]</t>
+          <t>39.0 [17.0,86.2]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.2]</t>
+          <t>32.0 [15.0,76.0]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>SpO2 (%, mean), median [Q1,Q3]</t>
+          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr"/>
       <c r="C80" t="n">
-        <v>19</v>
+        <v>5341</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>98.0 [96.3,99.2]</t>
+          <t>0.30 [0.14,0.50]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>97.2 [95.8,98.6]</t>
+          <t>0.26 [0.13,0.45]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>Heart Rate (mean), median [Q1,Q3]</t>
+          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr"/>
       <c r="C81" t="n">
-        <v>18</v>
+        <v>5341</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>87.5 [76.4,100.6]</t>
+          <t>2.0 [1.0,8.0]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>85.8 [75.8,97.9]</t>
+          <t>3.0 [1.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>PaO2 (min), median [Q1,Q3]</t>
+          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr"/>
       <c r="C82" t="n">
-        <v>4014</v>
+        <v>11653</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>88.5 [69.0,124.0]</t>
+          <t>16.0 [4.0,41.0]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>89.0 [72.0,118.0]</t>
+          <t>25.0 [5.5,63.0]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>PaCO2 (max), median [Q1,Q3]</t>
+          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B83" s="1" t="inlineStr"/>
       <c r="C83" t="n">
-        <v>4014</v>
+        <v>5827</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>44.0 [37.0,52.0]</t>
+          <t>3.0 [1.0,12.0]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>46.0 [39.0,53.0]</t>
+          <t>3.0 [1.0,10.0]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>pH (min), median [Q1,Q3]</t>
+          <t>VP_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B84" s="1" t="inlineStr"/>
       <c r="C84" t="n">
-        <v>2267</v>
+        <v>5827</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>7.3 [7.2,7.4]</t>
+          <t>29.0 [10.0,65.0]</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>7.3 [7.2,7.4]</t>
+          <t>29.0 [11.0,62.0]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>Glucose (max), median [Q1,Q3]</t>
+          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B85" s="1" t="inlineStr"/>
       <c r="C85" t="n">
-        <v>67</v>
+        <v>5827</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>154.0 [122.0,218.0]</t>
+          <t>0.23 [0.08,0.48]</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>147.0 [120.0,194.0]</t>
+          <t>0.25 [0.09,0.47]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>Sodium (min), median [Q1,Q3]</t>
+          <t>Respiratory Rate (mean), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B86" s="1" t="inlineStr"/>
       <c r="C86" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>137.0 [134.0,140.0]</t>
+          <t>19.4 [17.0,22.6]</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>137.0 [134.0,140.0]</t>
+          <t>19.1 [16.8,22.0]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>Potassium (max), median [Q1,Q3]</t>
+          <t>Mean Blood Pressure (mean), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B87" s="1" t="inlineStr"/>
       <c r="C87" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>4.5 [4.1,5.2]</t>
+          <t>77.5 [71.1,85.4]</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>4.5 [4.1,5.0]</t>
+          <t>74.7 [69.4,81.6]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>Cortisol (min), median [Q1,Q3]</t>
+          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B88" s="1" t="inlineStr"/>
       <c r="C88" t="n">
-        <v>12719</v>
+        <v>693</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>19.0 [13.5,30.9]</t>
+          <t>36.9 [36.6,37.3]</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>22.0 [12.5,33.9]</t>
+          <t>36.9 [36.6,37.2]</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Hemoglobin (min), median [Q1,Q3]</t>
+          <t>SpO2 (%, mean), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B89" s="1" t="inlineStr"/>
       <c r="C89" t="n">
-        <v>1753</v>
+        <v>19</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>9.8 [8.2,11.4]</t>
+          <t>98.0 [96.3,99.2]</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>10.0 [8.6,11.6]</t>
+          <t>97.2 [95.8,98.6]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>Fibrinogen (min), median [Q1,Q3]</t>
+          <t>Heart Rate (mean), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B90" s="1" t="inlineStr"/>
       <c r="C90" t="n">
-        <v>8424</v>
+        <v>18</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>226.0 [153.0,364.0]</t>
+          <t>87.5 [76.4,100.6]</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>228.5 [165.0,344.0]</t>
+          <t>85.8 [75.8,97.9]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>INR (max), median [Q1,Q3]</t>
+          <t>PaO2 (min), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B91" s="1" t="inlineStr"/>
       <c r="C91" t="n">
+        <v>4014</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>88.5 [69.0,124.0]</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>89.0 [72.0,118.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>PaCO2 (max), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr"/>
+      <c r="C92" t="n">
+        <v>4014</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>44.0 [37.0,52.0]</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>46.0 [39.0,53.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>pH (min), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr"/>
+      <c r="C93" t="n">
+        <v>2267</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>7.3 [7.2,7.4]</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>7.3 [7.2,7.4]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Glucose (max), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="inlineStr"/>
+      <c r="C94" t="n">
+        <v>67</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>154.0 [122.0,218.0]</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>147.0 [120.0,194.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Sodium (min), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="inlineStr"/>
+      <c r="C95" t="n">
+        <v>27</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>137.0 [134.0,140.0]</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>137.0 [134.0,140.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Potassium (max), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>34</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>4.5 [4.1,5.2]</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>4.5 [4.1,5.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Cortisol (min), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>12719</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>19.0 [13.5,30.9]</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>22.0 [12.5,33.9]</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Hemoglobin (min), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr"/>
+      <c r="C98" t="n">
+        <v>1753</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>9.8 [8.2,11.4]</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>10.0 [8.6,11.6]</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Fibrinogen (min), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>8424</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>226.0 [153.0,364.0]</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>228.5 [165.0,344.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>INR (max), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="inlineStr"/>
+      <c r="C100" t="n">
         <v>788</v>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>1.4 [1.2,1.7]</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E100" t="inlineStr">
         <is>
           <t>1.4 [1.2,1.7]</t>
         </is>
@@ -2447,10 +2672,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A32:A37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>